<commit_message>
fini les grilles aléatoires
</commit_message>
<xml_diff>
--- a/Journaux/JournalDeBord.xlsx
+++ b/Journaux/JournalDeBord.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Le sixième sprint a comencé</t>
+  </si>
+  <si>
+    <t>Le septième sprint a comencé</t>
   </si>
 </sst>
 </file>
@@ -349,8 +352,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:C10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="A1:C10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:C11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A1:C11">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -661,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,6 +772,15 @@
         <v>12</v>
       </c>
       <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>44643</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>